<commit_message>
Progress is ongoing on updating the codes and results according to the new data.
</commit_message>
<xml_diff>
--- a/result/Manchester/mandatory/Version2/Updated Results_27.06.2023.xlsx
+++ b/result/Manchester/mandatory/Version2/Updated Results_27.06.2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/tayebeh_saghapour_rmit_edu_au/Documents/Documents/travelDiaryProcessing/result/Manchester/mandatory/Version2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="776" documentId="8_{6F77D324-6248-40E6-B1F5-D6BEC9502B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B978CC2-7DD0-4002-BF79-45E951C9B3F8}"/>
+  <xr:revisionPtr revIDLastSave="779" documentId="8_{6F77D324-6248-40E6-B1F5-D6BEC9502B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73A64803-A414-432B-AECE-D77BE6BD3B9A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="2" activeTab="2" xr2:uid="{3D7712E4-13CC-45D5-A89D-D2EED1C8E686}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{3D7712E4-13CC-45D5-A89D-D2EED1C8E686}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -2403,7 +2403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2513,6 +2513,9 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2830,7 +2833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5902A00-30F1-49E6-A0FF-F139880F80EA}">
   <dimension ref="A1:CO89"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
@@ -15570,8 +15573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F7A2F2-2CC1-4D96-A417-88F7FA927B37}">
   <dimension ref="A1:AE141"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W78" sqref="W78"/>
+    <sheetView tabSelected="1" topLeftCell="J55" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64:K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19125,6 +19128,7 @@
       <c r="F65" s="9">
         <v>-1.14601</v>
       </c>
+      <c r="K65" s="60"/>
       <c r="M65" s="11" t="s">
         <v>507</v>
       </c>
@@ -19299,6 +19303,7 @@
       <c r="F68" s="9">
         <v>3.8535599999999999</v>
       </c>
+      <c r="K68" s="60"/>
       <c r="M68" s="11" t="s">
         <v>515</v>
       </c>
@@ -20733,7 +20738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C045ED-722A-4FCD-913F-84C88427D1B6}">
   <dimension ref="A1:AG69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P34" workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Results for descritionanry trips were also added.
</commit_message>
<xml_diff>
--- a/result/Manchester/mandatory/Version2/Updated Results_27.06.2023.xlsx
+++ b/result/Manchester/mandatory/Version2/Updated Results_27.06.2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rmiteduau-my.sharepoint.com/personal/tayebeh_saghapour_rmit_edu_au/Documents/Documents/travelDiaryProcessing/result/Manchester/mandatory/Version2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="987" documentId="8_{6F77D324-6248-40E6-B1F5-D6BEC9502B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C30648C-8B4D-4A6B-910C-B9893340D99E}"/>
+  <xr:revisionPtr revIDLastSave="988" documentId="8_{6F77D324-6248-40E6-B1F5-D6BEC9502B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D988A126-BAAF-4244-90F9-3F7C2352FEDC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{3D7712E4-13CC-45D5-A89D-D2EED1C8E686}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{3D7712E4-13CC-45D5-A89D-D2EED1C8E686}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="815">
   <si>
     <t>Estimate</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>Non-commute trips: Fast route-attributes (alpha = 9.2)</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -15860,7 +15863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F7A2F2-2CC1-4D96-A417-88F7FA927B37}">
   <dimension ref="A1:AD141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -17401,8 +17404,8 @@
       <c r="B22" s="67">
         <v>-1.1454899999999999</v>
       </c>
-      <c r="C22" s="67">
-        <v>0.35815000000000002</v>
+      <c r="C22" s="67" t="s">
+        <v>814</v>
       </c>
       <c r="D22" s="70" t="s">
         <v>564</v>
@@ -22936,7 +22939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C045ED-722A-4FCD-913F-84C88427D1B6}">
   <dimension ref="A1:AG69"/>
   <sheetViews>
-    <sheetView topLeftCell="P34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>

</xml_diff>